<commit_message>
Refactored FPL code into its own dir and created a new data import for PPL.
</commit_message>
<xml_diff>
--- a/poleams-conversion/src/main/resources/com/precisionhawk/poleams/processors/poleinspection/fpl/Survey_Report_Template.xlsx
+++ b/poleams-conversion/src/main/resources/com/precisionhawk/poleams/processors/poleinspection/fpl/Survey_Report_Template.xlsx
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1982" uniqueCount="481">
   <si>
     <t xml:space="preserve">Feeder:</t>
   </si>
@@ -1486,6 +1486,27 @@
   </si>
   <si>
     <t>156'</t>
+  </si>
+  <si>
+    <t>*3PH-TAN-Xarm-8' 6" Stl-35KV PT-E-6.0.1 F1</t>
+  </si>
+  <si>
+    <t>75'</t>
+  </si>
+  <si>
+    <t>139'</t>
+  </si>
+  <si>
+    <t>117'</t>
+  </si>
+  <si>
+    <t>3PH-TAN-Xarm-8' 6" Stl-35KV PT-E-6.0.1 F1</t>
+  </si>
+  <si>
+    <t>244'</t>
+  </si>
+  <si>
+    <t>30'</t>
   </si>
 </sst>
 </file>
@@ -6165,14 +6186,50 @@
       <c r="B59" t="n">
         <v>56.0</v>
       </c>
+      <c r="G59" t="n">
+        <v>40.0</v>
+      </c>
+      <c r="H59" t="s">
+        <v>184</v>
+      </c>
+      <c r="I59" t="s">
+        <v>474</v>
+      </c>
+      <c r="J59" t="s">
+        <v>475</v>
+      </c>
+      <c r="K59" t="s">
+        <v>476</v>
+      </c>
       <c r="P59" t="n">
         <v>0.0</v>
       </c>
       <c r="T59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="V59" t="n">
+        <v>20.25</v>
+      </c>
+      <c r="W59" t="n">
+        <v>1.5</v>
       </c>
       <c r="AH59" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="AJ59" t="n">
+        <v>19.170000076293945</v>
+      </c>
+      <c r="AK59" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AV59" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="AW59" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX59" t="s">
+        <v>167</v>
       </c>
       <c r="BD59" t="n">
         <v>25.999486923217773</v>
@@ -6181,7 +6238,10 @@
         <v>-80.4088134765625</v>
       </c>
       <c r="CD59" t="n">
-        <v>56.0</v>
+        <v>94.0</v>
+      </c>
+      <c r="CK59" t="n">
+        <v>69.0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7639,37 +7699,40 @@
         <v>45.0</v>
       </c>
       <c r="H80" t="s">
-        <v>173</v>
+        <v>417</v>
       </c>
       <c r="I80" t="s">
-        <v>327</v>
+        <v>436</v>
       </c>
       <c r="J80" t="s">
-        <v>350</v>
+        <v>477</v>
       </c>
       <c r="K80" t="s">
-        <v>345</v>
+        <v>335</v>
+      </c>
+      <c r="O80" t="s">
+        <v>391</v>
       </c>
       <c r="P80" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="T80" t="n">
         <v>1.0</v>
       </c>
       <c r="V80" t="n">
-        <v>22.329999923706055</v>
+        <v>19.079999923706055</v>
       </c>
       <c r="W80" t="n">
-        <v>1.0</v>
+        <v>1.5</v>
       </c>
       <c r="AH80" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="AJ80" t="n">
-        <v>20.75</v>
+        <v>18.079999923706055</v>
       </c>
       <c r="AK80" t="n">
-        <v>1.5</v>
+        <v>1.0</v>
       </c>
       <c r="AL80" t="n">
         <v>18.75</v>
@@ -7692,12 +7755,8 @@
       <c r="AX80" t="s">
         <v>167</v>
       </c>
-      <c r="AY80" t="s">
-        <v>324</v>
-      </c>
-      <c r="AZ80" t="n">
-        <v>1.0</v>
-      </c>
+      <c r="AY80"/>
+      <c r="AZ80"/>
       <c r="BD80" t="n">
         <v>26.007394790649414</v>
       </c>
@@ -7705,10 +7764,10 @@
         <v>-80.41071319580078</v>
       </c>
       <c r="CD80" t="n">
-        <v>77.0</v>
+        <v>199.0</v>
       </c>
       <c r="CK80" t="n">
-        <v>146.0</v>
+        <v>78.0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7805,40 +7864,49 @@
         <v>79.0</v>
       </c>
       <c r="G82" t="n">
-        <v>60.0</v>
+        <v>45.0</v>
       </c>
       <c r="H82" t="s">
         <v>417</v>
       </c>
       <c r="I82" t="s">
-        <v>418</v>
+        <v>478</v>
       </c>
       <c r="J82" t="s">
-        <v>420</v>
+        <v>479</v>
       </c>
       <c r="K82" t="s">
-        <v>422</v>
+        <v>346</v>
+      </c>
+      <c r="L82" t="s">
+        <v>480</v>
+      </c>
+      <c r="O82" t="s">
+        <v>205</v>
       </c>
       <c r="P82" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
+      </c>
+      <c r="R82" t="s">
+        <v>165</v>
       </c>
       <c r="T82" t="n">
         <v>1.0</v>
       </c>
       <c r="V82" t="n">
-        <v>20.0</v>
+        <v>19.25</v>
       </c>
       <c r="W82" t="n">
         <v>1.5</v>
       </c>
       <c r="AH82" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
       <c r="AJ82" t="n">
-        <v>27.5</v>
+        <v>18.170000076293945</v>
       </c>
       <c r="AK82" t="n">
-        <v>0.75</v>
+        <v>2.0</v>
       </c>
       <c r="AL82" t="n">
         <v>19.329999923706055</v>
@@ -7862,16 +7930,17 @@
         <v>3.0</v>
       </c>
       <c r="AW82" t="s">
-        <v>166</v>
+        <v>223</v>
       </c>
       <c r="AX82" t="s">
         <v>167</v>
       </c>
-      <c r="AY82" t="s">
-        <v>324</v>
-      </c>
+      <c r="AY82"/>
       <c r="AZ82" t="n">
         <v>1.0</v>
+      </c>
+      <c r="BA82" t="s">
+        <v>366</v>
       </c>
       <c r="BD82" t="n">
         <v>26.007396697998047</v>
@@ -7880,10 +7949,10 @@
         <v>-80.41143798828125</v>
       </c>
       <c r="CD82" t="n">
-        <v>79.0</v>
+        <v>95.0</v>
       </c>
       <c r="CK82" t="n">
-        <v>85.0</v>
+        <v>72.0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>